<commit_message>
Added more of Shinji's IF patches
</commit_message>
<xml_diff>
--- a/FO_patching.xlsx
+++ b/FO_patching.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="449" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="449" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="2015-097" sheetId="1" state="visible" r:id="rId2"/>
@@ -14,13 +14,14 @@
     <sheet name="2015-139" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="2015-161" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="2016-013" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="Winter2016" sheetId="7" state="visible" r:id="rId8"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="53">
   <si>
     <t>Band</t>
   </si>
@@ -165,6 +166,21 @@
   <si>
     <t>PSR3-1</t>
   </si>
+  <si>
+    <t>Summer 2016</t>
+  </si>
+  <si>
+    <t>PSR4-0</t>
+  </si>
+  <si>
+    <t>PSR4-1</t>
+  </si>
+  <si>
+    <t>PSR4-2</t>
+  </si>
+  <si>
+    <t>PSR4-3</t>
+  </si>
 </sst>
 </file>
 
@@ -173,7 +189,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -202,8 +218,22 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF3333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF009900"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -214,6 +244,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFE6E6E6"/>
         <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -258,7 +294,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="32">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -351,6 +387,42 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -364,14 +436,14 @@
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFE6E6E6"/>
-      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FFFF3333"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF009900"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
@@ -4606,8 +4678,8 @@
   </sheetPr>
   <dimension ref="A1:M42"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -5649,6 +5721,1170 @@
       <c r="K42" s="17"/>
       <c r="L42" s="15"/>
       <c r="M42" s="15"/>
+    </row>
+  </sheetData>
+  <mergeCells count="35">
+    <mergeCell ref="A3:A10"/>
+    <mergeCell ref="B3:B6"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="A11:A18"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="B15:B18"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="A19:A26"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="B23:B26"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="A27:A34"/>
+    <mergeCell ref="B27:B30"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="B31:B34"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="A35:A42"/>
+    <mergeCell ref="B35:B38"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="B39:B42"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="C41:C42"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:N42"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q45" activeCellId="0" sqref="Q45"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="24.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="N1" s="22" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" s="14"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="15"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="23" t="n">
+        <v>18</v>
+      </c>
+      <c r="B3" s="23" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="25"/>
+      <c r="F3" s="23" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" s="23" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3" s="23"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="26"/>
+      <c r="K3" s="26"/>
+      <c r="L3" s="25"/>
+      <c r="M3" s="23"/>
+      <c r="N3" s="23"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="23"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="25"/>
+      <c r="F4" s="23" t="n">
+        <v>2</v>
+      </c>
+      <c r="G4" s="23" t="n">
+        <v>2</v>
+      </c>
+      <c r="H4" s="23"/>
+      <c r="I4" s="26"/>
+      <c r="J4" s="26"/>
+      <c r="K4" s="26"/>
+      <c r="L4" s="25"/>
+      <c r="M4" s="23"/>
+      <c r="N4" s="23"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="23"/>
+      <c r="B5" s="23"/>
+      <c r="C5" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="25"/>
+      <c r="F5" s="23" t="n">
+        <v>3</v>
+      </c>
+      <c r="G5" s="23" t="n">
+        <v>3</v>
+      </c>
+      <c r="H5" s="23"/>
+      <c r="I5" s="23"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="25"/>
+      <c r="L5" s="25"/>
+      <c r="M5" s="23"/>
+      <c r="N5" s="23"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="23"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="25"/>
+      <c r="F6" s="23" t="n">
+        <v>4</v>
+      </c>
+      <c r="G6" s="23" t="n">
+        <v>4</v>
+      </c>
+      <c r="H6" s="23"/>
+      <c r="I6" s="23"/>
+      <c r="J6" s="23"/>
+      <c r="K6" s="25"/>
+      <c r="L6" s="25"/>
+      <c r="M6" s="23"/>
+      <c r="N6" s="23"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="23"/>
+      <c r="B7" s="23" t="n">
+        <v>2</v>
+      </c>
+      <c r="C7" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="25"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="23"/>
+      <c r="I7" s="23"/>
+      <c r="J7" s="23"/>
+      <c r="K7" s="25"/>
+      <c r="L7" s="25"/>
+      <c r="M7" s="23"/>
+      <c r="N7" s="23"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="23"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="25"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="23"/>
+      <c r="J8" s="23"/>
+      <c r="K8" s="25"/>
+      <c r="L8" s="25"/>
+      <c r="M8" s="23"/>
+      <c r="N8" s="23"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="23"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="25"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="23"/>
+      <c r="I9" s="23"/>
+      <c r="J9" s="23"/>
+      <c r="K9" s="25"/>
+      <c r="L9" s="25"/>
+      <c r="M9" s="23"/>
+      <c r="N9" s="23"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="23"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="25"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="23"/>
+      <c r="I10" s="23"/>
+      <c r="J10" s="23"/>
+      <c r="K10" s="25"/>
+      <c r="L10" s="25"/>
+      <c r="M10" s="23"/>
+      <c r="N10" s="23"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="15" t="n">
+        <v>20</v>
+      </c>
+      <c r="B11" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15" t="n">
+        <v>14</v>
+      </c>
+      <c r="L11" s="17"/>
+      <c r="M11" s="15"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="15"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="17" t="n">
+        <v>2</v>
+      </c>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="18" t="n">
+        <v>10</v>
+      </c>
+      <c r="J12" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="K12" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="L12" s="17"/>
+      <c r="M12" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="N12" s="15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="15"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="17" t="n">
+        <v>3</v>
+      </c>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="15" t="n">
+        <v>16</v>
+      </c>
+      <c r="K13" s="17"/>
+      <c r="L13" s="17"/>
+      <c r="M13" s="27"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="15"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="17" t="n">
+        <v>4</v>
+      </c>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="15" t="n">
+        <v>12</v>
+      </c>
+      <c r="J14" s="28" t="n">
+        <v>2</v>
+      </c>
+      <c r="K14" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="L14" s="17"/>
+      <c r="M14" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="N14" s="15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="15"/>
+      <c r="B15" s="15" t="n">
+        <v>2</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="17" t="n">
+        <v>5</v>
+      </c>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="15"/>
+      <c r="K15" s="17"/>
+      <c r="L15" s="17"/>
+      <c r="M15" s="27"/>
+      <c r="N15" s="15"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="15"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="17" t="n">
+        <v>6</v>
+      </c>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="15"/>
+      <c r="J16" s="15" t="n">
+        <v>3</v>
+      </c>
+      <c r="K16" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="L16" s="17"/>
+      <c r="M16" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="N16" s="15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="15"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="17" t="n">
+        <v>7</v>
+      </c>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="15"/>
+      <c r="K17" s="17"/>
+      <c r="L17" s="17"/>
+      <c r="M17" s="29"/>
+      <c r="N17" s="15"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="15"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" s="17" t="n">
+        <v>8</v>
+      </c>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
+      <c r="I18" s="15"/>
+      <c r="J18" s="15" t="n">
+        <v>4</v>
+      </c>
+      <c r="K18" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="L18" s="17"/>
+      <c r="M18" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="N18" s="15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="15" t="n">
+        <v>22</v>
+      </c>
+      <c r="B19" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" s="12" t="n">
+        <v>9</v>
+      </c>
+      <c r="F19" s="18" t="n">
+        <v>5</v>
+      </c>
+      <c r="G19" s="18" t="n">
+        <v>5</v>
+      </c>
+      <c r="H19" s="18" t="n">
+        <v>1</v>
+      </c>
+      <c r="I19" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="J19" s="15" t="n">
+        <v>5</v>
+      </c>
+      <c r="K19" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="M19" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="N19" s="15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="15"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" s="17" t="n">
+        <v>10</v>
+      </c>
+      <c r="F20" s="15" t="n">
+        <v>6</v>
+      </c>
+      <c r="G20" s="15" t="n">
+        <v>6</v>
+      </c>
+      <c r="H20" s="15" t="n">
+        <v>2</v>
+      </c>
+      <c r="I20" s="15" t="n">
+        <v>2</v>
+      </c>
+      <c r="J20" s="15" t="n">
+        <v>6</v>
+      </c>
+      <c r="K20" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="L20" s="20"/>
+      <c r="M20" s="30"/>
+      <c r="N20" s="15" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="15"/>
+      <c r="B21" s="15"/>
+      <c r="C21" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" s="17" t="n">
+        <v>11</v>
+      </c>
+      <c r="F21" s="15" t="n">
+        <v>7</v>
+      </c>
+      <c r="G21" s="15" t="n">
+        <v>7</v>
+      </c>
+      <c r="H21" s="15" t="n">
+        <v>3</v>
+      </c>
+      <c r="I21" s="15" t="n">
+        <v>3</v>
+      </c>
+      <c r="J21" s="15" t="n">
+        <v>7</v>
+      </c>
+      <c r="K21" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="L21" s="20"/>
+      <c r="M21" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="N21" s="15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="15"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" s="12" t="n">
+        <v>12</v>
+      </c>
+      <c r="F22" s="18" t="n">
+        <v>8</v>
+      </c>
+      <c r="G22" s="18" t="n">
+        <v>8</v>
+      </c>
+      <c r="H22" s="18" t="n">
+        <v>4</v>
+      </c>
+      <c r="I22" s="15" t="n">
+        <v>4</v>
+      </c>
+      <c r="J22" s="15" t="n">
+        <v>8</v>
+      </c>
+      <c r="K22" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="M22" s="30"/>
+      <c r="N22" s="15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="15"/>
+      <c r="B23" s="15" t="n">
+        <v>2</v>
+      </c>
+      <c r="C23" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" s="17" t="n">
+        <v>13</v>
+      </c>
+      <c r="F23" s="15"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="15" t="n">
+        <v>5</v>
+      </c>
+      <c r="I23" s="18" t="n">
+        <v>5</v>
+      </c>
+      <c r="J23" s="15" t="n">
+        <v>9</v>
+      </c>
+      <c r="L23" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="M23" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="N23" s="15"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="15"/>
+      <c r="B24" s="15"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" s="12" t="n">
+        <v>14</v>
+      </c>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="18" t="n">
+        <v>6</v>
+      </c>
+      <c r="I24" s="15" t="n">
+        <v>6</v>
+      </c>
+      <c r="J24" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="K24" s="19"/>
+      <c r="L24" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="M24" s="31"/>
+      <c r="N24" s="15"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="15"/>
+      <c r="B25" s="15"/>
+      <c r="C25" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E25" s="12" t="n">
+        <v>15</v>
+      </c>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="18" t="n">
+        <v>7</v>
+      </c>
+      <c r="I25" s="15" t="n">
+        <v>7</v>
+      </c>
+      <c r="J25" s="28" t="n">
+        <v>11</v>
+      </c>
+      <c r="K25" s="19"/>
+      <c r="L25" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="M25" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="N25" s="15"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="15"/>
+      <c r="B26" s="15"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" s="17" t="n">
+        <v>16</v>
+      </c>
+      <c r="F26" s="15"/>
+      <c r="G26" s="15"/>
+      <c r="H26" s="15" t="n">
+        <v>8</v>
+      </c>
+      <c r="I26" s="18" t="n">
+        <v>8</v>
+      </c>
+      <c r="J26" s="15" t="n">
+        <v>12</v>
+      </c>
+      <c r="L26" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="N26" s="15"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="15" t="n">
+        <v>24</v>
+      </c>
+      <c r="B27" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="C27" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E27" s="17"/>
+      <c r="F27" s="15" t="n">
+        <v>9</v>
+      </c>
+      <c r="G27" s="15" t="n">
+        <v>9</v>
+      </c>
+      <c r="H27" s="15" t="n">
+        <v>9</v>
+      </c>
+      <c r="I27" s="15" t="n">
+        <v>9</v>
+      </c>
+      <c r="L27" s="17"/>
+      <c r="M27" s="15"/>
+      <c r="N27" s="15" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="15"/>
+      <c r="B28" s="15"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E28" s="17"/>
+      <c r="F28" s="15" t="n">
+        <v>10</v>
+      </c>
+      <c r="G28" s="15" t="n">
+        <v>10</v>
+      </c>
+      <c r="H28" s="15" t="n">
+        <v>10</v>
+      </c>
+      <c r="I28" s="15" t="n">
+        <v>13</v>
+      </c>
+      <c r="L28" s="17"/>
+      <c r="M28" s="15"/>
+      <c r="N28" s="15" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="15"/>
+      <c r="B29" s="15"/>
+      <c r="C29" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E29" s="17"/>
+      <c r="F29" s="15" t="n">
+        <v>11</v>
+      </c>
+      <c r="G29" s="15" t="n">
+        <v>11</v>
+      </c>
+      <c r="H29" s="15" t="n">
+        <v>11</v>
+      </c>
+      <c r="I29" s="18" t="n">
+        <v>11</v>
+      </c>
+      <c r="K29" s="17"/>
+      <c r="L29" s="17"/>
+      <c r="M29" s="15"/>
+      <c r="N29" s="15" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="15"/>
+      <c r="B30" s="15"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E30" s="17"/>
+      <c r="F30" s="15" t="n">
+        <v>12</v>
+      </c>
+      <c r="G30" s="15" t="n">
+        <v>12</v>
+      </c>
+      <c r="H30" s="15" t="n">
+        <v>12</v>
+      </c>
+      <c r="I30" s="15" t="n">
+        <v>15</v>
+      </c>
+      <c r="K30" s="17"/>
+      <c r="L30" s="17"/>
+      <c r="M30" s="15"/>
+      <c r="N30" s="15" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="15"/>
+      <c r="B31" s="15" t="n">
+        <v>2</v>
+      </c>
+      <c r="C31" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D31" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E31" s="17"/>
+      <c r="F31" s="15"/>
+      <c r="G31" s="15"/>
+      <c r="H31" s="15"/>
+      <c r="I31" s="15"/>
+      <c r="J31" s="15"/>
+      <c r="K31" s="17"/>
+      <c r="L31" s="17"/>
+      <c r="M31" s="15"/>
+      <c r="N31" s="15"/>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="15"/>
+      <c r="B32" s="15"/>
+      <c r="C32" s="15"/>
+      <c r="D32" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E32" s="17"/>
+      <c r="F32" s="15"/>
+      <c r="G32" s="15"/>
+      <c r="H32" s="15"/>
+      <c r="I32" s="15"/>
+      <c r="J32" s="15"/>
+      <c r="K32" s="17"/>
+      <c r="L32" s="17"/>
+      <c r="M32" s="15"/>
+      <c r="N32" s="15"/>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="15"/>
+      <c r="B33" s="15"/>
+      <c r="C33" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D33" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E33" s="17"/>
+      <c r="F33" s="15"/>
+      <c r="G33" s="15"/>
+      <c r="H33" s="15"/>
+      <c r="I33" s="15"/>
+      <c r="J33" s="15"/>
+      <c r="K33" s="17"/>
+      <c r="L33" s="17"/>
+      <c r="M33" s="15"/>
+      <c r="N33" s="15"/>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="15"/>
+      <c r="B34" s="15"/>
+      <c r="C34" s="15"/>
+      <c r="D34" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E34" s="17"/>
+      <c r="F34" s="15"/>
+      <c r="G34" s="15"/>
+      <c r="H34" s="15"/>
+      <c r="I34" s="15"/>
+      <c r="J34" s="15"/>
+      <c r="K34" s="17"/>
+      <c r="L34" s="17"/>
+      <c r="M34" s="15"/>
+      <c r="N34" s="15"/>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="15" t="n">
+        <v>26</v>
+      </c>
+      <c r="B35" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="C35" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D35" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E35" s="17"/>
+      <c r="F35" s="15" t="n">
+        <v>13</v>
+      </c>
+      <c r="G35" s="15" t="n">
+        <v>13</v>
+      </c>
+      <c r="H35" s="15" t="n">
+        <v>13</v>
+      </c>
+      <c r="I35" s="20"/>
+      <c r="J35" s="15" t="n">
+        <v>13</v>
+      </c>
+      <c r="K35" s="20"/>
+      <c r="L35" s="17"/>
+      <c r="M35" s="15"/>
+      <c r="N35" s="15" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="15"/>
+      <c r="B36" s="15"/>
+      <c r="C36" s="15"/>
+      <c r="D36" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E36" s="17"/>
+      <c r="F36" s="15" t="n">
+        <v>14</v>
+      </c>
+      <c r="G36" s="15" t="n">
+        <v>14</v>
+      </c>
+      <c r="H36" s="15" t="n">
+        <v>14</v>
+      </c>
+      <c r="I36" s="20"/>
+      <c r="J36" s="15" t="n">
+        <v>14</v>
+      </c>
+      <c r="K36" s="20"/>
+      <c r="L36" s="17"/>
+      <c r="M36" s="15"/>
+      <c r="N36" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="15"/>
+      <c r="B37" s="15"/>
+      <c r="C37" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D37" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E37" s="17"/>
+      <c r="F37" s="15" t="n">
+        <v>15</v>
+      </c>
+      <c r="G37" s="15" t="n">
+        <v>15</v>
+      </c>
+      <c r="H37" s="15" t="n">
+        <v>15</v>
+      </c>
+      <c r="I37" s="15"/>
+      <c r="J37" s="28" t="n">
+        <v>15</v>
+      </c>
+      <c r="K37" s="17"/>
+      <c r="L37" s="17"/>
+      <c r="M37" s="15"/>
+      <c r="N37" s="15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="15"/>
+      <c r="B38" s="15"/>
+      <c r="C38" s="15"/>
+      <c r="D38" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E38" s="17"/>
+      <c r="F38" s="15" t="n">
+        <v>16</v>
+      </c>
+      <c r="G38" s="15" t="n">
+        <v>16</v>
+      </c>
+      <c r="H38" s="15" t="n">
+        <v>16</v>
+      </c>
+      <c r="I38" s="15"/>
+      <c r="J38" s="15" t="n">
+        <v>16</v>
+      </c>
+      <c r="K38" s="17"/>
+      <c r="L38" s="17"/>
+      <c r="M38" s="15"/>
+      <c r="N38" s="15" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="15"/>
+      <c r="B39" s="15" t="n">
+        <v>2</v>
+      </c>
+      <c r="C39" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D39" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E39" s="17"/>
+      <c r="F39" s="15"/>
+      <c r="G39" s="15"/>
+      <c r="H39" s="15"/>
+      <c r="I39" s="15"/>
+      <c r="J39" s="15"/>
+      <c r="K39" s="17"/>
+      <c r="L39" s="17"/>
+      <c r="M39" s="15"/>
+      <c r="N39" s="15"/>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="15"/>
+      <c r="B40" s="15"/>
+      <c r="C40" s="15"/>
+      <c r="D40" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E40" s="17"/>
+      <c r="F40" s="15"/>
+      <c r="G40" s="15"/>
+      <c r="H40" s="15"/>
+      <c r="I40" s="15"/>
+      <c r="J40" s="15"/>
+      <c r="K40" s="17"/>
+      <c r="L40" s="17"/>
+      <c r="M40" s="15"/>
+      <c r="N40" s="15"/>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="15"/>
+      <c r="B41" s="15"/>
+      <c r="C41" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D41" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E41" s="17"/>
+      <c r="F41" s="15"/>
+      <c r="G41" s="15"/>
+      <c r="H41" s="15"/>
+      <c r="I41" s="15"/>
+      <c r="J41" s="15"/>
+      <c r="K41" s="17"/>
+      <c r="L41" s="17"/>
+      <c r="M41" s="15"/>
+      <c r="N41" s="15"/>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="15"/>
+      <c r="B42" s="15"/>
+      <c r="C42" s="15"/>
+      <c r="D42" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E42" s="17"/>
+      <c r="F42" s="15"/>
+      <c r="G42" s="15"/>
+      <c r="H42" s="15"/>
+      <c r="I42" s="15"/>
+      <c r="J42" s="15"/>
+      <c r="K42" s="17"/>
+      <c r="L42" s="17"/>
+      <c r="M42" s="15"/>
+      <c r="N42" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="35">

</xml_diff>

<commit_message>
Renamed last CDSCC IF patch ssheet
</commit_message>
<xml_diff>
--- a/FO_patching.xlsx
+++ b/FO_patching.xlsx
@@ -14,7 +14,7 @@
     <sheet name="2015-139" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="2015-161" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="2016-013" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="Winter2016" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="2016-126" sheetId="7" state="visible" r:id="rId8"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
@@ -294,7 +294,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="31">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -407,10 +407,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -6117,7 +6113,7 @@
       <c r="I14" s="15" t="n">
         <v>12</v>
       </c>
-      <c r="J14" s="28" t="n">
+      <c r="J14" s="15" t="n">
         <v>2</v>
       </c>
       <c r="K14" s="17" t="s">
@@ -6200,7 +6196,7 @@
       <c r="I17" s="15"/>
       <c r="K17" s="17"/>
       <c r="L17" s="17"/>
-      <c r="M17" s="29"/>
+      <c r="M17" s="28"/>
       <c r="N17" s="15"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6265,7 +6261,7 @@
       <c r="K19" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="M19" s="30" t="s">
+      <c r="M19" s="29" t="s">
         <v>40</v>
       </c>
       <c r="N19" s="15" t="s">
@@ -6301,7 +6297,7 @@
         <v>27</v>
       </c>
       <c r="L20" s="20"/>
-      <c r="M20" s="30"/>
+      <c r="M20" s="29"/>
       <c r="N20" s="15" t="s">
         <v>37</v>
       </c>
@@ -6337,7 +6333,7 @@
         <v>24</v>
       </c>
       <c r="L21" s="20"/>
-      <c r="M21" s="30" t="s">
+      <c r="M21" s="29" t="s">
         <v>41</v>
       </c>
       <c r="N21" s="15" t="s">
@@ -6372,7 +6368,7 @@
       <c r="K22" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="M22" s="30"/>
+      <c r="M22" s="29"/>
       <c r="N22" s="15" t="s">
         <v>39</v>
       </c>
@@ -6405,7 +6401,7 @@
       <c r="L23" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="M23" s="30" t="s">
+      <c r="M23" s="29" t="s">
         <v>42</v>
       </c>
       <c r="N23" s="15"/>
@@ -6435,7 +6431,7 @@
       <c r="L24" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="M24" s="31"/>
+      <c r="M24" s="30"/>
       <c r="N24" s="15"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6458,14 +6454,14 @@
       <c r="I25" s="15" t="n">
         <v>7</v>
       </c>
-      <c r="J25" s="28" t="n">
+      <c r="J25" s="15" t="n">
         <v>11</v>
       </c>
       <c r="K25" s="19"/>
       <c r="L25" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="M25" s="30" t="s">
+      <c r="M25" s="29" t="s">
         <v>43</v>
       </c>
       <c r="N25" s="15"/>
@@ -6770,7 +6766,7 @@
         <v>15</v>
       </c>
       <c r="I37" s="15"/>
-      <c r="J37" s="28" t="n">
+      <c r="J37" s="15" t="n">
         <v>15</v>
       </c>
       <c r="K37" s="17"/>

</xml_diff>

<commit_message>
changed patching to SAO
</commit_message>
<xml_diff>
--- a/FO_patching.xlsx
+++ b/FO_patching.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="995" firstSheet="0" activeTab="7"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="2015-097" sheetId="1" state="visible" r:id="rId2"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="743" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="742" uniqueCount="89">
   <si>
     <t xml:space="preserve">Band</t>
   </si>
@@ -649,19 +649,19 @@
   </sheetPr>
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="Q:Q A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.22448979591837"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.56122448979592"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.36224489795918"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.7755102040816"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="12.9591836734694"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="7.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="12.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="12.96"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1285,7 +1285,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1300,18 +1300,18 @@
   </sheetPr>
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="Q:Q A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.22448979591837"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.63775510204082"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="6.27040816326531"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="12.9591836734694"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="6.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="12.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="12.96"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1935,7 +1935,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1950,20 +1950,20 @@
   </sheetPr>
   <dimension ref="A1:J42"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J25" activeCellId="1" sqref="Q:Q J25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J25" activeCellId="0" sqref="J25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.1734693877551"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="6.27040816326531"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="5" width="8.63775510204082"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="12.9591836734694"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="6.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="12.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="0" width="12.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="5" width="8.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="12.96"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="24.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2852,7 +2852,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2867,23 +2867,23 @@
   </sheetPr>
   <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K1" activeCellId="1" sqref="Q:Q K1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K1" activeCellId="0" sqref="K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.1938775510204"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.22448979591837"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="5.73469387755102"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="4" width="5.73469387755102"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="4" width="8.63775510204082"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="11" width="8.63775510204082"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="11" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="11" width="8.63775510204082"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="5" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="5" width="8.63775510204082"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.77551020408163"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="5.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="4" width="5.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="4" width="8.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="11" width="8.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="11" width="16.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="11" width="8.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="5" width="13.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="5" width="8.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="8.79"/>
   </cols>
   <sheetData>
     <row r="1" s="6" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3832,7 +3832,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -3847,21 +3847,21 @@
   </sheetPr>
   <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G18" activeCellId="1" sqref="Q:Q G18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G18" activeCellId="0" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.1938775510204"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.22448979591837"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="5.73469387755102"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="8.63775510204082"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="8.63775510204082"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="5" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="5" width="8.63775510204082"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="12.9591836734694"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="5.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="8.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="0" width="8.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="5" width="13.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="5" width="8.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="12.96"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4810,7 +4810,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -4825,22 +4825,22 @@
   </sheetPr>
   <dimension ref="A1:M42"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="Q:Q A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.1938775510204"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.24489795918367"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="5.73469387755102"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="8.63775510204082"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="8.63775510204082"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="5" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="5" width="8.63775510204082"/>
-    <col collapsed="false" hidden="false" max="13" min="12" style="11" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="12.9591836734694"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="5.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="8.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="0" width="8.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="5" width="13.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="5" width="8.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="11" width="10.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="14" style="0" width="12.96"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="24.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5909,7 +5909,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -5924,19 +5924,19 @@
   </sheetPr>
   <dimension ref="A1:N42"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N42" activeCellId="1" sqref="Q:Q N42"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N42" activeCellId="0" sqref="N42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.92857142857143"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.1428571428571"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.41836734693878"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.14795918367347"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="12.8979591836735"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="12.8979591836735"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="6.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="6.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="12.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="12.9"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="24.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7079,7 +7079,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -7094,27 +7094,27 @@
   </sheetPr>
   <dimension ref="A1:Q46"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q1" activeCellId="0" sqref="Q:Q"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.53061224489796"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.98979591836735"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="4.62755102040816"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="5.35714285714286"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="7.66836734693878"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.1581632653061"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.1785714285714"/>
-    <col collapsed="false" hidden="false" max="11" min="9" style="0" width="12.2142857142857"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.13775510204082"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="9.32142857142857"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="9.18877551020408"/>
-    <col collapsed="false" hidden="false" max="16" min="15" style="0" width="8.65816326530612"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="5" width="12.2142857142857"/>
-    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="12.2142857142857"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="4.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="5.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="7.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="9" style="0" width="12.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="8.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="9.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="9.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="15" style="0" width="8.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="5" width="12.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="18" style="0" width="12.21"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7179,15 +7179,14 @@
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
       <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
+      <c r="G2" s="13" t="n">
+        <v>1</v>
+      </c>
       <c r="H2" s="13"/>
-      <c r="I2" s="14" t="s">
-        <v>15</v>
-      </c>
       <c r="J2" s="14"/>
       <c r="K2" s="8"/>
       <c r="L2" s="8"/>
-      <c r="M2" s="15"/>
+      <c r="M2" s="14"/>
       <c r="N2" s="15"/>
       <c r="O2" s="33"/>
       <c r="P2" s="34"/>
@@ -8468,7 +8467,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>